<commit_message>
changes a trashcan and a lamp
that were trapping kos
</commit_message>
<xml_diff>
--- a/Assets/levelMapincludingCollectables.xlsx
+++ b/Assets/levelMapincludingCollectables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="19">
   <si>
     <t>{"g"</t>
   </si>
@@ -80,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -174,7 +174,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -189,7 +189,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -5283,8 +5283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="AC31" sqref="AC31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15"/>
@@ -8404,7 +8404,7 @@
       <c r="AB31" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AC31" s="6">
+      <c r="AC31" s="6" t="s">
         <v>4</v>
       </c>
       <c r="AD31" s="15" t="s">

</xml_diff>

<commit_message>
added lamp in the beginning of the maze
added first battery in the lamp to trigger "Mom words"
</commit_message>
<xml_diff>
--- a/Assets/levelMapincludingCollectables.xlsx
+++ b/Assets/levelMapincludingCollectables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="19">
   <si>
     <t>{"g"</t>
   </si>
@@ -5283,8 +5283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="AC31" sqref="AC31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15"/>
@@ -5394,8 +5394,8 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>7</v>
+      <c r="B2" s="4">
+        <v>2</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>1</v>
@@ -5495,7 +5495,7 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3" s="1">
@@ -7118,7 +7118,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -7218,8 +7218,8 @@
       <c r="C20" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="6">
-        <v>4</v>
+      <c r="D20" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -7427,10 +7427,10 @@
         <v>1</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="G22" s="6">
+        <v>4</v>
       </c>
       <c r="H22" s="7">
         <v>3</v>

</xml_diff>